<commit_message>
removed coordinate dropdown in infinium run template?
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Experiment_run_Infinium_v4_13_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Experiment_run_Infinium_v4_13_0.xlsx
@@ -53674,10 +53674,6 @@
     </row>
   </sheetData>
   <dataValidations count="8">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D5:D101" type="list">
-      <formula1>#ref!</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G100 F101" type="list">
       <formula1>Index!$D$2:$D$25</formula1>
       <formula2>0</formula2>
@@ -53704,6 +53700,10 @@
     </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G9" type="list">
       <formula1>INDIRECT(SUBSTITUTE(INDEX(Experiments!$D$7:$D$100, MATCH($A9,Experiments!$A$7:$A$100,0))," ","_"))</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D5:D101" type="none">
+      <formula1>#REF!</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
correct coordinate spec for infinium (#899)
* correct coordinate spec for infinium

* removed coordinate dropdown in infinium run template?
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Experiment_run_Infinium_v4_13_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Experiment_run_Infinium_v4_13_0.xlsx
@@ -53674,10 +53674,6 @@
     </row>
   </sheetData>
   <dataValidations count="8">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D5:D101" type="list">
-      <formula1>#ref!</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G100 F101" type="list">
       <formula1>Index!$D$2:$D$25</formula1>
       <formula2>0</formula2>
@@ -53704,6 +53700,10 @@
     </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G9" type="list">
       <formula1>INDIRECT(SUBSTITUTE(INDEX(Experiments!$D$7:$D$100, MATCH($A9,Experiments!$A$7:$A$100,0))," ","_"))</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D5:D101" type="none">
+      <formula1>#REF!</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>

</xml_diff>